<commit_message>
atualizei os requisitos e o quem somos
</commit_message>
<xml_diff>
--- a/documentacao/requisitos/sprint_backlog.xlsx
+++ b/documentacao/requisitos/sprint_backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PI\grupo9-ads\documentacao\requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510428CF-2D25-40A2-8738-E01AB933769A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B635EEE-C3B6-4026-905C-6C0A933E8C9E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,10 +16,16 @@
     <sheet name="Sprint Backlog 1" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint Backlog 2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -285,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -369,13 +375,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -383,73 +383,73 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -766,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,10 +784,10 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C1"/>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="37"/>
+      <c r="F1" s="57"/>
     </row>
     <row r="2" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -836,10 +836,10 @@
       <c r="AE2" s="6"/>
     </row>
     <row r="3" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="40">
+      <c r="B3" s="49">
         <v>100</v>
       </c>
       <c r="C3" s="16"/>
@@ -860,8 +860,8 @@
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
-      <c r="B4" s="40"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="49"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17" t="s">
         <v>11</v>
@@ -880,8 +880,8 @@
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="41"/>
+      <c r="A5" s="53"/>
+      <c r="B5" s="50"/>
       <c r="C5" s="19"/>
       <c r="D5" s="20" t="s">
         <v>13</v>
@@ -900,10 +900,10 @@
       </c>
     </row>
     <row r="6" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="43">
+      <c r="B6" s="48">
         <v>100</v>
       </c>
       <c r="C6" s="22"/>
@@ -918,11 +918,12 @@
       </c>
       <c r="G6" s="24"/>
       <c r="H6" s="4"/>
+      <c r="J6" s="47"/>
       <c r="K6" s="12"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A7" s="38"/>
-      <c r="B7" s="40"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="49"/>
       <c r="C7" s="16"/>
       <c r="D7" s="17" t="s">
         <v>11</v>
@@ -937,8 +938,8 @@
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A8" s="38"/>
-      <c r="B8" s="40"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="49"/>
       <c r="C8" s="16"/>
       <c r="D8" s="17" t="s">
         <v>17</v>
@@ -953,8 +954,8 @@
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A9" s="39"/>
-      <c r="B9" s="41"/>
+      <c r="A9" s="53"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="19"/>
       <c r="D9" s="20" t="s">
         <v>18</v>
@@ -989,10 +990,10 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:31" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="43">
+      <c r="B11" s="48">
         <v>50</v>
       </c>
       <c r="C11" s="22"/>
@@ -1009,8 +1010,8 @@
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A12" s="38"/>
-      <c r="B12" s="40"/>
+      <c r="A12" s="52"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="16"/>
       <c r="D12" s="17" t="s">
         <v>22</v>
@@ -1025,8 +1026,8 @@
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
-      <c r="B13" s="40"/>
+      <c r="A13" s="52"/>
+      <c r="B13" s="49"/>
       <c r="C13" s="16"/>
       <c r="D13" s="17" t="s">
         <v>23</v>
@@ -1041,8 +1042,8 @@
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
-      <c r="B14" s="41"/>
+      <c r="A14" s="53"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="19"/>
       <c r="D14" s="20" t="s">
         <v>24</v>
@@ -1057,10 +1058,10 @@
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="43">
+      <c r="B15" s="48">
         <v>90</v>
       </c>
       <c r="C15" s="22"/>
@@ -1077,8 +1078,8 @@
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A16" s="38"/>
-      <c r="B16" s="40"/>
+      <c r="A16" s="52"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="16"/>
       <c r="D16" s="17" t="s">
         <v>23</v>
@@ -1093,8 +1094,8 @@
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
-      <c r="B17" s="41"/>
+      <c r="A17" s="53"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="19"/>
       <c r="D17" s="20" t="s">
         <v>35</v>
@@ -1105,14 +1106,14 @@
       <c r="F17" s="20">
         <v>2</v>
       </c>
-      <c r="G17" s="31"/>
+      <c r="G17" s="21"/>
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="43">
+      <c r="B18" s="48">
         <v>100</v>
       </c>
       <c r="C18" s="22"/>
@@ -1125,12 +1126,12 @@
       <c r="F18" s="23">
         <v>3</v>
       </c>
-      <c r="G18" s="32"/>
+      <c r="G18" s="31"/>
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="38"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="52"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="16"/>
       <c r="D19" s="17" t="s">
         <v>23</v>
@@ -1141,12 +1142,12 @@
       <c r="F19" s="17">
         <v>2</v>
       </c>
-      <c r="G19" s="33"/>
+      <c r="G19" s="18"/>
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="39"/>
-      <c r="B20" s="41"/>
+      <c r="A20" s="53"/>
+      <c r="B20" s="50"/>
       <c r="C20" s="19"/>
       <c r="D20" s="20" t="s">
         <v>34</v>
@@ -1154,15 +1155,17 @@
       <c r="E20" s="20">
         <v>2</v>
       </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
+      <c r="F20" s="20">
+        <v>1</v>
+      </c>
+      <c r="G20" s="21"/>
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="43">
+      <c r="B21" s="48">
         <v>100</v>
       </c>
       <c r="C21" s="22"/>
@@ -1179,36 +1182,40 @@
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="38"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="34"/>
+      <c r="A22" s="52"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="32"/>
       <c r="D22" s="17" t="s">
         <v>23</v>
       </c>
       <c r="E22" s="17">
         <v>2</v>
       </c>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
+      <c r="F22" s="17">
+        <v>2</v>
+      </c>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="39"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="35"/>
+      <c r="A23" s="53"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="33"/>
       <c r="D23" s="20" t="s">
         <v>34</v>
       </c>
       <c r="E23" s="20">
         <v>3</v>
       </c>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
+      <c r="F23" s="20">
+        <v>2</v>
+      </c>
+      <c r="G23" s="21"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="44" t="s">
+      <c r="A24" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="43">
+      <c r="B24" s="48">
         <v>30</v>
       </c>
       <c r="C24" s="22"/>
@@ -1224,8 +1231,8 @@
       <c r="G24" s="24"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="45"/>
-      <c r="B25" s="40"/>
+      <c r="A25" s="55"/>
+      <c r="B25" s="49"/>
       <c r="C25" s="16"/>
       <c r="D25" s="17" t="s">
         <v>23</v>
@@ -1236,11 +1243,11 @@
       <c r="F25" s="17">
         <v>4</v>
       </c>
-      <c r="G25" s="33"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="46"/>
-      <c r="B26" s="41"/>
+      <c r="A26" s="56"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="19"/>
       <c r="D26" s="20" t="s">
         <v>34</v>
@@ -1248,14 +1255,16 @@
       <c r="E26" s="20">
         <v>2</v>
       </c>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
+      <c r="F26" s="20">
+        <v>1</v>
+      </c>
+      <c r="G26" s="21"/>
     </row>
     <row r="27" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="43">
+      <c r="B27" s="48">
         <v>20</v>
       </c>
       <c r="C27" s="22"/>
@@ -1268,11 +1277,11 @@
       <c r="F27" s="23">
         <v>3</v>
       </c>
-      <c r="G27" s="36"/>
+      <c r="G27" s="34"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="38"/>
-      <c r="B28" s="40"/>
+      <c r="A28" s="52"/>
+      <c r="B28" s="49"/>
       <c r="C28" s="16"/>
       <c r="D28" s="17" t="s">
         <v>23</v>
@@ -1286,8 +1295,8 @@
       <c r="G28" s="18"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="39"/>
-      <c r="B29" s="41"/>
+      <c r="A29" s="53"/>
+      <c r="B29" s="50"/>
       <c r="C29" s="19"/>
       <c r="D29" s="20" t="s">
         <v>34</v>
@@ -1295,14 +1304,16 @@
       <c r="E29" s="20">
         <v>2</v>
       </c>
-      <c r="F29" s="20"/>
-      <c r="G29" s="31"/>
+      <c r="F29" s="36">
+        <v>1</v>
+      </c>
+      <c r="G29" s="21"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="42" t="s">
+      <c r="A30" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="43">
+      <c r="B30" s="48">
         <v>100</v>
       </c>
       <c r="C30" s="22"/>
@@ -1318,8 +1329,8 @@
       <c r="G30" s="24"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="38"/>
-      <c r="B31" s="40"/>
+      <c r="A31" s="52"/>
+      <c r="B31" s="49"/>
       <c r="C31" s="16"/>
       <c r="D31" s="17" t="s">
         <v>32</v>
@@ -1333,8 +1344,8 @@
       <c r="G31" s="18"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="39"/>
-      <c r="B32" s="41"/>
+      <c r="A32" s="53"/>
+      <c r="B32" s="50"/>
       <c r="C32" s="19"/>
       <c r="D32" s="20" t="s">
         <v>33</v>
@@ -1415,6 +1426,17 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="A21:A23"/>
@@ -1423,17 +1445,6 @@
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="B27:B29"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1445,7 +1456,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,10 +1470,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="37"/>
+      <c r="F1" s="57"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -1489,10 +1500,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="40">
+      <c r="B3" s="49">
         <v>100</v>
       </c>
       <c r="C3" s="16"/>
@@ -1503,12 +1514,12 @@
         <v>1</v>
       </c>
       <c r="F3" s="17"/>
-      <c r="G3" s="47"/>
+      <c r="G3" s="35"/>
       <c r="H3" s="17"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
-      <c r="B4" s="40"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="49"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17" t="s">
         <v>38</v>
@@ -1517,12 +1528,12 @@
         <v>2</v>
       </c>
       <c r="F4" s="17"/>
-      <c r="G4" s="47"/>
+      <c r="G4" s="35"/>
       <c r="H4" s="17"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="38"/>
-      <c r="B5" s="40"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="49"/>
       <c r="C5" s="16"/>
       <c r="D5" s="17" t="s">
         <v>39</v>
@@ -1531,12 +1542,12 @@
         <v>1</v>
       </c>
       <c r="F5" s="17"/>
-      <c r="G5" s="47"/>
+      <c r="G5" s="35"/>
       <c r="H5" s="17"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="38"/>
-      <c r="B6" s="40"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="49"/>
       <c r="C6" s="16"/>
       <c r="D6" s="17" t="s">
         <v>40</v>
@@ -1545,12 +1556,12 @@
         <v>1</v>
       </c>
       <c r="F6" s="17"/>
-      <c r="G6" s="47"/>
+      <c r="G6" s="35"/>
       <c r="H6" s="17"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="39"/>
-      <c r="B7" s="41"/>
+      <c r="A7" s="53"/>
+      <c r="B7" s="50"/>
       <c r="C7" s="19"/>
       <c r="D7" s="20" t="s">
         <v>41</v>
@@ -1559,14 +1570,14 @@
         <v>3</v>
       </c>
       <c r="F7" s="20"/>
-      <c r="G7" s="48"/>
+      <c r="G7" s="36"/>
       <c r="H7" s="20"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="43">
+      <c r="B8" s="48">
         <v>100</v>
       </c>
       <c r="C8" s="22"/>
@@ -1577,12 +1588,12 @@
         <v>2</v>
       </c>
       <c r="F8" s="23"/>
-      <c r="G8" s="58"/>
+      <c r="G8" s="46"/>
       <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="38"/>
-      <c r="B9" s="40"/>
+      <c r="A9" s="52"/>
+      <c r="B9" s="49"/>
       <c r="C9" s="16"/>
       <c r="D9" s="13" t="s">
         <v>45</v>
@@ -1591,12 +1602,12 @@
         <v>3</v>
       </c>
       <c r="F9" s="17"/>
-      <c r="G9" s="47"/>
+      <c r="G9" s="35"/>
       <c r="H9" s="17"/>
     </row>
     <row r="10" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="40"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="49"/>
       <c r="C10" s="16"/>
       <c r="D10" s="13" t="s">
         <v>46</v>
@@ -1605,12 +1616,12 @@
         <v>1</v>
       </c>
       <c r="F10" s="17"/>
-      <c r="G10" s="47"/>
+      <c r="G10" s="35"/>
       <c r="H10" s="17"/>
     </row>
     <row r="11" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
-      <c r="B11" s="41"/>
+      <c r="A11" s="53"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="19"/>
       <c r="D11" s="15" t="s">
         <v>41</v>
@@ -1619,7 +1630,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="20"/>
-      <c r="G11" s="48"/>
+      <c r="G11" s="36"/>
       <c r="H11" s="20"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1629,7 +1640,7 @@
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
       <c r="F12" s="17"/>
-      <c r="G12" s="47"/>
+      <c r="G12" s="35"/>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1639,7 +1650,7 @@
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
-      <c r="G13" s="47"/>
+      <c r="G13" s="35"/>
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1649,7 +1660,7 @@
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
-      <c r="G14" s="47"/>
+      <c r="G14" s="35"/>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1659,7 +1670,7 @@
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
-      <c r="G15" s="47"/>
+      <c r="G15" s="35"/>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1669,7 +1680,7 @@
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
-      <c r="G16" s="47"/>
+      <c r="G16" s="35"/>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1679,9 +1690,9 @@
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
-      <c r="G17" s="47"/>
+      <c r="G17" s="35"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="59"/>
+      <c r="I17" s="47"/>
     </row>
     <row r="18" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
@@ -1690,7 +1701,7 @@
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
-      <c r="G18" s="49"/>
+      <c r="G18" s="37"/>
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1700,7 +1711,7 @@
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
-      <c r="G19" s="47"/>
+      <c r="G19" s="35"/>
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1710,7 +1721,7 @@
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
-      <c r="G20" s="47"/>
+      <c r="G20" s="35"/>
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1720,28 +1731,28 @@
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
-      <c r="G21" s="47"/>
+      <c r="G21" s="35"/>
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="17"/>
-      <c r="C22" s="56"/>
+      <c r="C22" s="44"/>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="57"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="45"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="17"/>
-      <c r="C23" s="56"/>
+      <c r="C23" s="44"/>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="57"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="45"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
@@ -1750,8 +1761,8 @@
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="57"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="45"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
@@ -1760,71 +1771,71 @@
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="57"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="45"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="51"/>
-      <c r="B26" s="54"/>
+      <c r="A26" s="39"/>
+      <c r="B26" s="42"/>
       <c r="C26" s="16"/>
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
-      <c r="G26" s="47"/>
+      <c r="G26" s="35"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="52"/>
-      <c r="B27" s="54"/>
+      <c r="A27" s="40"/>
+      <c r="B27" s="42"/>
       <c r="C27" s="16"/>
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
       <c r="F27" s="17"/>
-      <c r="G27" s="50"/>
+      <c r="G27" s="38"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="52"/>
-      <c r="B28" s="54"/>
+      <c r="A28" s="40"/>
+      <c r="B28" s="42"/>
       <c r="C28" s="16"/>
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
       <c r="F28" s="17"/>
-      <c r="G28" s="47"/>
+      <c r="G28" s="35"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="52"/>
-      <c r="B29" s="54"/>
+      <c r="A29" s="40"/>
+      <c r="B29" s="42"/>
       <c r="C29" s="16"/>
       <c r="D29" s="17"/>
       <c r="E29" s="17"/>
       <c r="F29" s="17"/>
-      <c r="G29" s="47"/>
+      <c r="G29" s="35"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="52"/>
-      <c r="B30" s="54"/>
+      <c r="A30" s="40"/>
+      <c r="B30" s="42"/>
       <c r="C30" s="16"/>
       <c r="D30" s="17"/>
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
-      <c r="G30" s="47"/>
+      <c r="G30" s="35"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="52"/>
-      <c r="B31" s="54"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="42"/>
       <c r="C31" s="16"/>
       <c r="D31" s="17"/>
       <c r="E31" s="17"/>
       <c r="F31" s="17"/>
-      <c r="G31" s="47"/>
+      <c r="G31" s="35"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="53"/>
-      <c r="B32" s="55"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="43"/>
       <c r="C32" s="19"/>
       <c r="D32" s="20"/>
       <c r="E32" s="20"/>
       <c r="F32" s="20"/>
-      <c r="G32" s="48"/>
+      <c r="G32" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
adição de itens na sprint backlog 2
</commit_message>
<xml_diff>
--- a/documentacao/requisitos/sprint_backlog.xlsx
+++ b/documentacao/requisitos/sprint_backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PI\grupo9-ads\documentacao\requisitos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\princesa\Documents\Bandtec\GIT-Bandtec\grupo9-ads\documentacao\requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B635EEE-C3B6-4026-905C-6C0A933E8C9E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CB5972-0247-401B-B081-2EAD93A78C66}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint Backlog 1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
   <si>
     <t>(em dias)</t>
   </si>
@@ -173,6 +173,24 @@
   </si>
   <si>
     <t>Revisar conectividade com o site</t>
+  </si>
+  <si>
+    <t>banco de dados</t>
+  </si>
+  <si>
+    <t>Criar banco de dados para os dados das geladeiras</t>
+  </si>
+  <si>
+    <t>Conectar arduino ao banco de dados</t>
+  </si>
+  <si>
+    <t>Conectar bando de dados ao site</t>
+  </si>
+  <si>
+    <t>Fazer o teste de captação de dados</t>
+  </si>
+  <si>
+    <t>Checar se os dados estao sendo salvos corretamente</t>
   </si>
 </sst>
 </file>
@@ -291,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -420,8 +438,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -432,11 +456,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -447,8 +468,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -766,7 +787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE43"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -784,10 +805,10 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C1"/>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="57"/>
+      <c r="F1" s="48"/>
     </row>
     <row r="2" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -836,10 +857,10 @@
       <c r="AE2" s="6"/>
     </row>
     <row r="3" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="49">
+      <c r="B3" s="51">
         <v>100</v>
       </c>
       <c r="C3" s="16"/>
@@ -860,8 +881,8 @@
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
-      <c r="B4" s="49"/>
+      <c r="A4" s="49"/>
+      <c r="B4" s="51"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17" t="s">
         <v>11</v>
@@ -880,8 +901,8 @@
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="50"/>
+      <c r="A5" s="50"/>
+      <c r="B5" s="52"/>
       <c r="C5" s="19"/>
       <c r="D5" s="20" t="s">
         <v>13</v>
@@ -900,10 +921,10 @@
       </c>
     </row>
     <row r="6" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="48">
+      <c r="B6" s="54">
         <v>100</v>
       </c>
       <c r="C6" s="22"/>
@@ -922,8 +943,8 @@
       <c r="K6" s="12"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A7" s="52"/>
-      <c r="B7" s="49"/>
+      <c r="A7" s="49"/>
+      <c r="B7" s="51"/>
       <c r="C7" s="16"/>
       <c r="D7" s="17" t="s">
         <v>11</v>
@@ -938,8 +959,8 @@
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A8" s="52"/>
-      <c r="B8" s="49"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="51"/>
       <c r="C8" s="16"/>
       <c r="D8" s="17" t="s">
         <v>17</v>
@@ -954,8 +975,8 @@
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A9" s="53"/>
-      <c r="B9" s="50"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="52"/>
       <c r="C9" s="19"/>
       <c r="D9" s="20" t="s">
         <v>18</v>
@@ -990,10 +1011,10 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:31" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="48">
+      <c r="B11" s="54">
         <v>50</v>
       </c>
       <c r="C11" s="22"/>
@@ -1010,8 +1031,8 @@
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A12" s="52"/>
-      <c r="B12" s="49"/>
+      <c r="A12" s="49"/>
+      <c r="B12" s="51"/>
       <c r="C12" s="16"/>
       <c r="D12" s="17" t="s">
         <v>22</v>
@@ -1026,8 +1047,8 @@
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="52"/>
-      <c r="B13" s="49"/>
+      <c r="A13" s="49"/>
+      <c r="B13" s="51"/>
       <c r="C13" s="16"/>
       <c r="D13" s="17" t="s">
         <v>23</v>
@@ -1042,8 +1063,8 @@
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A14" s="53"/>
-      <c r="B14" s="50"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="52"/>
       <c r="C14" s="19"/>
       <c r="D14" s="20" t="s">
         <v>24</v>
@@ -1058,10 +1079,10 @@
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A15" s="51" t="s">
+      <c r="A15" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="48">
+      <c r="B15" s="54">
         <v>90</v>
       </c>
       <c r="C15" s="22"/>
@@ -1078,8 +1099,8 @@
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A16" s="52"/>
-      <c r="B16" s="49"/>
+      <c r="A16" s="49"/>
+      <c r="B16" s="51"/>
       <c r="C16" s="16"/>
       <c r="D16" s="17" t="s">
         <v>23</v>
@@ -1094,8 +1115,8 @@
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="53"/>
-      <c r="B17" s="50"/>
+      <c r="A17" s="50"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="19"/>
       <c r="D17" s="20" t="s">
         <v>35</v>
@@ -1110,10 +1131,10 @@
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="51" t="s">
+      <c r="A18" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="48">
+      <c r="B18" s="54">
         <v>100</v>
       </c>
       <c r="C18" s="22"/>
@@ -1130,8 +1151,8 @@
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="52"/>
-      <c r="B19" s="49"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="51"/>
       <c r="C19" s="16"/>
       <c r="D19" s="17" t="s">
         <v>23</v>
@@ -1146,8 +1167,8 @@
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="53"/>
-      <c r="B20" s="50"/>
+      <c r="A20" s="50"/>
+      <c r="B20" s="52"/>
       <c r="C20" s="19"/>
       <c r="D20" s="20" t="s">
         <v>34</v>
@@ -1162,10 +1183,10 @@
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="51" t="s">
+      <c r="A21" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="48">
+      <c r="B21" s="54">
         <v>100</v>
       </c>
       <c r="C21" s="22"/>
@@ -1182,8 +1203,8 @@
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="52"/>
-      <c r="B22" s="49"/>
+      <c r="A22" s="49"/>
+      <c r="B22" s="51"/>
       <c r="C22" s="32"/>
       <c r="D22" s="17" t="s">
         <v>23</v>
@@ -1197,8 +1218,8 @@
       <c r="G22" s="18"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="53"/>
-      <c r="B23" s="50"/>
+      <c r="A23" s="50"/>
+      <c r="B23" s="52"/>
       <c r="C23" s="33"/>
       <c r="D23" s="20" t="s">
         <v>34</v>
@@ -1212,10 +1233,10 @@
       <c r="G23" s="21"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="54" t="s">
+      <c r="A24" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="48">
+      <c r="B24" s="54">
         <v>30</v>
       </c>
       <c r="C24" s="22"/>
@@ -1231,8 +1252,8 @@
       <c r="G24" s="24"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="55"/>
-      <c r="B25" s="49"/>
+      <c r="A25" s="56"/>
+      <c r="B25" s="51"/>
       <c r="C25" s="16"/>
       <c r="D25" s="17" t="s">
         <v>23</v>
@@ -1246,8 +1267,8 @@
       <c r="G25" s="18"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="56"/>
-      <c r="B26" s="50"/>
+      <c r="A26" s="57"/>
+      <c r="B26" s="52"/>
       <c r="C26" s="19"/>
       <c r="D26" s="20" t="s">
         <v>34</v>
@@ -1261,10 +1282,10 @@
       <c r="G26" s="21"/>
     </row>
     <row r="27" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="51" t="s">
+      <c r="A27" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="48">
+      <c r="B27" s="54">
         <v>20</v>
       </c>
       <c r="C27" s="22"/>
@@ -1280,8 +1301,8 @@
       <c r="G27" s="34"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="52"/>
-      <c r="B28" s="49"/>
+      <c r="A28" s="49"/>
+      <c r="B28" s="51"/>
       <c r="C28" s="16"/>
       <c r="D28" s="17" t="s">
         <v>23</v>
@@ -1295,8 +1316,8 @@
       <c r="G28" s="18"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="53"/>
-      <c r="B29" s="50"/>
+      <c r="A29" s="50"/>
+      <c r="B29" s="52"/>
       <c r="C29" s="19"/>
       <c r="D29" s="20" t="s">
         <v>34</v>
@@ -1310,10 +1331,10 @@
       <c r="G29" s="21"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="48">
+      <c r="B30" s="54">
         <v>100</v>
       </c>
       <c r="C30" s="22"/>
@@ -1329,8 +1350,8 @@
       <c r="G30" s="24"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="52"/>
-      <c r="B31" s="49"/>
+      <c r="A31" s="49"/>
+      <c r="B31" s="51"/>
       <c r="C31" s="16"/>
       <c r="D31" s="17" t="s">
         <v>32</v>
@@ -1344,8 +1365,8 @@
       <c r="G31" s="18"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="53"/>
-      <c r="B32" s="50"/>
+      <c r="A32" s="50"/>
+      <c r="B32" s="52"/>
       <c r="C32" s="19"/>
       <c r="D32" s="20" t="s">
         <v>33</v>
@@ -1426,17 +1447,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B18:B20"/>
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="A21:A23"/>
@@ -1445,6 +1455,17 @@
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1456,7 +1477,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,10 +1491,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="57"/>
+      <c r="F1" s="48"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -1500,10 +1521,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="49">
+      <c r="B3" s="51">
         <v>100</v>
       </c>
       <c r="C3" s="16"/>
@@ -1518,8 +1539,8 @@
       <c r="H3" s="17"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
-      <c r="B4" s="49"/>
+      <c r="A4" s="49"/>
+      <c r="B4" s="51"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17" t="s">
         <v>38</v>
@@ -1532,8 +1553,8 @@
       <c r="H4" s="17"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
-      <c r="B5" s="49"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="51"/>
       <c r="C5" s="16"/>
       <c r="D5" s="17" t="s">
         <v>39</v>
@@ -1546,8 +1567,8 @@
       <c r="H5" s="17"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="52"/>
-      <c r="B6" s="49"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="51"/>
       <c r="C6" s="16"/>
       <c r="D6" s="17" t="s">
         <v>40</v>
@@ -1560,8 +1581,8 @@
       <c r="H6" s="17"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="53"/>
-      <c r="B7" s="50"/>
+      <c r="A7" s="50"/>
+      <c r="B7" s="52"/>
       <c r="C7" s="19"/>
       <c r="D7" s="20" t="s">
         <v>41</v>
@@ -1574,10 +1595,10 @@
       <c r="H7" s="20"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="48">
+      <c r="B8" s="54">
         <v>100</v>
       </c>
       <c r="C8" s="22"/>
@@ -1592,8 +1613,8 @@
       <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
-      <c r="B9" s="49"/>
+      <c r="A9" s="49"/>
+      <c r="B9" s="51"/>
       <c r="C9" s="16"/>
       <c r="D9" s="13" t="s">
         <v>45</v>
@@ -1606,8 +1627,8 @@
       <c r="H9" s="17"/>
     </row>
     <row r="10" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="52"/>
-      <c r="B10" s="49"/>
+      <c r="A10" s="49"/>
+      <c r="B10" s="51"/>
       <c r="C10" s="16"/>
       <c r="D10" s="13" t="s">
         <v>46</v>
@@ -1620,8 +1641,8 @@
       <c r="H10" s="17"/>
     </row>
     <row r="11" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="53"/>
-      <c r="B11" s="50"/>
+      <c r="A11" s="50"/>
+      <c r="B11" s="52"/>
       <c r="C11" s="19"/>
       <c r="D11" s="15" t="s">
         <v>41</v>
@@ -1634,61 +1655,89 @@
       <c r="H11" s="20"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="17"/>
+      <c r="A12" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="54">
+        <v>100</v>
+      </c>
       <c r="C12" s="16"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
+      <c r="D12" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="58">
+        <v>2</v>
+      </c>
       <c r="F12" s="17"/>
       <c r="G12" s="35"/>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="17"/>
+      <c r="A13" s="49"/>
+      <c r="B13" s="51"/>
       <c r="C13" s="16"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
+      <c r="D13" s="58" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="17">
+        <v>3</v>
+      </c>
       <c r="F13" s="17"/>
       <c r="G13" s="35"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="17"/>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="49"/>
+      <c r="B14" s="51"/>
       <c r="C14" s="16"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
+      <c r="D14" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="17">
+        <v>2</v>
+      </c>
       <c r="F14" s="17"/>
       <c r="G14" s="35"/>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="17"/>
+      <c r="A15" s="49"/>
+      <c r="B15" s="51"/>
       <c r="C15" s="16"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
+      <c r="D15" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="17">
+        <v>1</v>
+      </c>
       <c r="F15" s="17"/>
       <c r="G15" s="35"/>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="17"/>
+      <c r="A16" s="49"/>
+      <c r="B16" s="51"/>
       <c r="C16" s="16"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
+      <c r="D16" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="17">
+        <v>1</v>
+      </c>
       <c r="F16" s="17"/>
       <c r="G16" s="35"/>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="17"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="51"/>
       <c r="C17" s="16"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
+      <c r="D17" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="17">
+        <v>2</v>
+      </c>
       <c r="F17" s="17"/>
       <c r="G17" s="35"/>
       <c r="H17" s="4"/>
@@ -1838,7 +1887,9 @@
       <c r="G32" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="A12:A17"/>
     <mergeCell ref="B8:B11"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="A3:A7"/>
@@ -1846,6 +1897,6 @@
     <mergeCell ref="A8:A11"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Melhorias na monografia 2
</commit_message>
<xml_diff>
--- a/documentacao/requisitos/sprint_backlog.xlsx
+++ b/documentacao/requisitos/sprint_backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giuli\Desktop\projeto backup  31052019\documentacao\requisitos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vitória Cristina\Desktop\grupo9-ads\documentacao\requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CF80D3-266C-40FC-A487-261353D5BFA8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E693598D-34BA-4ED2-866C-714ED02FB10C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -175,9 +175,6 @@
     <t>Revisar conectividade com o site</t>
   </si>
   <si>
-    <t>banco de dados</t>
-  </si>
-  <si>
     <t>Criar banco de dados para os dados das geladeiras</t>
   </si>
   <si>
@@ -191,6 +188,9 @@
   </si>
   <si>
     <t>Checar se os dados estao sendo salvos corretamente</t>
+  </si>
+  <si>
+    <t>Banco de dados</t>
   </si>
 </sst>
 </file>
@@ -438,8 +438,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -450,11 +459,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -464,12 +470,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -787,7 +787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -805,10 +805,10 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C1"/>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="57"/>
+      <c r="F1" s="49"/>
     </row>
     <row r="2" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -857,10 +857,10 @@
       <c r="AE2" s="6"/>
     </row>
     <row r="3" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="49">
+      <c r="B3" s="52">
         <v>100</v>
       </c>
       <c r="C3" s="16"/>
@@ -881,8 +881,8 @@
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
-      <c r="B4" s="49"/>
+      <c r="A4" s="50"/>
+      <c r="B4" s="52"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17" t="s">
         <v>11</v>
@@ -901,8 +901,8 @@
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="50"/>
+      <c r="A5" s="51"/>
+      <c r="B5" s="53"/>
       <c r="C5" s="19"/>
       <c r="D5" s="20" t="s">
         <v>13</v>
@@ -921,10 +921,10 @@
       </c>
     </row>
     <row r="6" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="48">
+      <c r="B6" s="55">
         <v>100</v>
       </c>
       <c r="C6" s="22"/>
@@ -943,8 +943,8 @@
       <c r="K6" s="12"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A7" s="52"/>
-      <c r="B7" s="49"/>
+      <c r="A7" s="50"/>
+      <c r="B7" s="52"/>
       <c r="C7" s="16"/>
       <c r="D7" s="17" t="s">
         <v>11</v>
@@ -959,8 +959,8 @@
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A8" s="52"/>
-      <c r="B8" s="49"/>
+      <c r="A8" s="50"/>
+      <c r="B8" s="52"/>
       <c r="C8" s="16"/>
       <c r="D8" s="17" t="s">
         <v>17</v>
@@ -975,8 +975,8 @@
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A9" s="53"/>
-      <c r="B9" s="50"/>
+      <c r="A9" s="51"/>
+      <c r="B9" s="53"/>
       <c r="C9" s="19"/>
       <c r="D9" s="20" t="s">
         <v>18</v>
@@ -1011,10 +1011,10 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:31" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="48">
+      <c r="B11" s="55">
         <v>50</v>
       </c>
       <c r="C11" s="22"/>
@@ -1031,8 +1031,8 @@
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A12" s="52"/>
-      <c r="B12" s="49"/>
+      <c r="A12" s="50"/>
+      <c r="B12" s="52"/>
       <c r="C12" s="16"/>
       <c r="D12" s="17" t="s">
         <v>22</v>
@@ -1047,8 +1047,8 @@
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="52"/>
-      <c r="B13" s="49"/>
+      <c r="A13" s="50"/>
+      <c r="B13" s="52"/>
       <c r="C13" s="16"/>
       <c r="D13" s="17" t="s">
         <v>23</v>
@@ -1063,8 +1063,8 @@
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A14" s="53"/>
-      <c r="B14" s="50"/>
+      <c r="A14" s="51"/>
+      <c r="B14" s="53"/>
       <c r="C14" s="19"/>
       <c r="D14" s="20" t="s">
         <v>24</v>
@@ -1079,10 +1079,10 @@
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A15" s="51" t="s">
+      <c r="A15" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="48">
+      <c r="B15" s="55">
         <v>90</v>
       </c>
       <c r="C15" s="22"/>
@@ -1099,8 +1099,8 @@
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A16" s="52"/>
-      <c r="B16" s="49"/>
+      <c r="A16" s="50"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="16"/>
       <c r="D16" s="17" t="s">
         <v>23</v>
@@ -1115,8 +1115,8 @@
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="53"/>
-      <c r="B17" s="50"/>
+      <c r="A17" s="51"/>
+      <c r="B17" s="53"/>
       <c r="C17" s="19"/>
       <c r="D17" s="20" t="s">
         <v>35</v>
@@ -1131,10 +1131,10 @@
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="51" t="s">
+      <c r="A18" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="48">
+      <c r="B18" s="55">
         <v>100</v>
       </c>
       <c r="C18" s="22"/>
@@ -1151,8 +1151,8 @@
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="52"/>
-      <c r="B19" s="49"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="52"/>
       <c r="C19" s="16"/>
       <c r="D19" s="17" t="s">
         <v>23</v>
@@ -1167,8 +1167,8 @@
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="53"/>
-      <c r="B20" s="50"/>
+      <c r="A20" s="51"/>
+      <c r="B20" s="53"/>
       <c r="C20" s="19"/>
       <c r="D20" s="20" t="s">
         <v>34</v>
@@ -1183,10 +1183,10 @@
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="51" t="s">
+      <c r="A21" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="48">
+      <c r="B21" s="55">
         <v>100</v>
       </c>
       <c r="C21" s="22"/>
@@ -1203,8 +1203,8 @@
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="52"/>
-      <c r="B22" s="49"/>
+      <c r="A22" s="50"/>
+      <c r="B22" s="52"/>
       <c r="C22" s="32"/>
       <c r="D22" s="17" t="s">
         <v>23</v>
@@ -1218,8 +1218,8 @@
       <c r="G22" s="18"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="53"/>
-      <c r="B23" s="50"/>
+      <c r="A23" s="51"/>
+      <c r="B23" s="53"/>
       <c r="C23" s="33"/>
       <c r="D23" s="20" t="s">
         <v>34</v>
@@ -1233,10 +1233,10 @@
       <c r="G23" s="21"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="54" t="s">
+      <c r="A24" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="48">
+      <c r="B24" s="55">
         <v>30</v>
       </c>
       <c r="C24" s="22"/>
@@ -1252,8 +1252,8 @@
       <c r="G24" s="24"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="55"/>
-      <c r="B25" s="49"/>
+      <c r="A25" s="57"/>
+      <c r="B25" s="52"/>
       <c r="C25" s="16"/>
       <c r="D25" s="17" t="s">
         <v>23</v>
@@ -1267,8 +1267,8 @@
       <c r="G25" s="18"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="56"/>
-      <c r="B26" s="50"/>
+      <c r="A26" s="58"/>
+      <c r="B26" s="53"/>
       <c r="C26" s="19"/>
       <c r="D26" s="20" t="s">
         <v>34</v>
@@ -1282,10 +1282,10 @@
       <c r="G26" s="21"/>
     </row>
     <row r="27" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="51" t="s">
+      <c r="A27" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="48">
+      <c r="B27" s="55">
         <v>20</v>
       </c>
       <c r="C27" s="22"/>
@@ -1301,8 +1301,8 @@
       <c r="G27" s="34"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="52"/>
-      <c r="B28" s="49"/>
+      <c r="A28" s="50"/>
+      <c r="B28" s="52"/>
       <c r="C28" s="16"/>
       <c r="D28" s="17" t="s">
         <v>23</v>
@@ -1316,8 +1316,8 @@
       <c r="G28" s="18"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="53"/>
-      <c r="B29" s="50"/>
+      <c r="A29" s="51"/>
+      <c r="B29" s="53"/>
       <c r="C29" s="19"/>
       <c r="D29" s="20" t="s">
         <v>34</v>
@@ -1331,10 +1331,10 @@
       <c r="G29" s="21"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="48">
+      <c r="B30" s="55">
         <v>100</v>
       </c>
       <c r="C30" s="22"/>
@@ -1350,8 +1350,8 @@
       <c r="G30" s="24"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="52"/>
-      <c r="B31" s="49"/>
+      <c r="A31" s="50"/>
+      <c r="B31" s="52"/>
       <c r="C31" s="16"/>
       <c r="D31" s="17" t="s">
         <v>32</v>
@@ -1365,8 +1365,8 @@
       <c r="G31" s="18"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="53"/>
-      <c r="B32" s="50"/>
+      <c r="A32" s="51"/>
+      <c r="B32" s="53"/>
       <c r="C32" s="19"/>
       <c r="D32" s="20" t="s">
         <v>33</v>
@@ -1447,17 +1447,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B18:B20"/>
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="A21:A23"/>
@@ -1466,6 +1455,17 @@
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1477,7 +1477,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1491,10 +1491,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="57"/>
+      <c r="F1" s="49"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -1521,10 +1521,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="49">
+      <c r="B3" s="52">
         <v>100</v>
       </c>
       <c r="C3" s="16"/>
@@ -1541,8 +1541,8 @@
       <c r="H3" s="17"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
-      <c r="B4" s="49"/>
+      <c r="A4" s="50"/>
+      <c r="B4" s="52"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17" t="s">
         <v>38</v>
@@ -1557,8 +1557,8 @@
       <c r="H4" s="17"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
-      <c r="B5" s="49"/>
+      <c r="A5" s="50"/>
+      <c r="B5" s="52"/>
       <c r="C5" s="16"/>
       <c r="D5" s="17" t="s">
         <v>39</v>
@@ -1573,8 +1573,8 @@
       <c r="H5" s="17"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="52"/>
-      <c r="B6" s="49"/>
+      <c r="A6" s="50"/>
+      <c r="B6" s="52"/>
       <c r="C6" s="16"/>
       <c r="D6" s="17" t="s">
         <v>40</v>
@@ -1589,8 +1589,8 @@
       <c r="H6" s="17"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="53"/>
-      <c r="B7" s="50"/>
+      <c r="A7" s="51"/>
+      <c r="B7" s="53"/>
       <c r="C7" s="19"/>
       <c r="D7" s="20" t="s">
         <v>41</v>
@@ -1605,10 +1605,10 @@
       <c r="H7" s="20"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="48">
+      <c r="B8" s="55">
         <v>100</v>
       </c>
       <c r="C8" s="22"/>
@@ -1621,12 +1621,12 @@
       <c r="F8" s="23">
         <v>4</v>
       </c>
-      <c r="G8" s="58"/>
+      <c r="G8" s="48"/>
       <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
-      <c r="B9" s="49"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="52"/>
       <c r="C9" s="16"/>
       <c r="D9" s="13" t="s">
         <v>45</v>
@@ -1641,8 +1641,8 @@
       <c r="H9" s="17"/>
     </row>
     <row r="10" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="52"/>
-      <c r="B10" s="49"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="52"/>
       <c r="C10" s="16"/>
       <c r="D10" s="13" t="s">
         <v>46</v>
@@ -1657,8 +1657,8 @@
       <c r="H10" s="17"/>
     </row>
     <row r="11" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="53"/>
-      <c r="B11" s="50"/>
+      <c r="A11" s="51"/>
+      <c r="B11" s="53"/>
       <c r="C11" s="19"/>
       <c r="D11" s="15" t="s">
         <v>41</v>
@@ -1673,15 +1673,15 @@
       <c r="H11" s="20"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="48">
+      <c r="A12" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="55">
         <v>100</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" s="47">
         <v>2</v>
@@ -1693,11 +1693,11 @@
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="52"/>
-      <c r="B13" s="49"/>
+      <c r="A13" s="50"/>
+      <c r="B13" s="52"/>
       <c r="C13" s="16"/>
       <c r="D13" s="47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E13" s="17">
         <v>3</v>
@@ -1709,11 +1709,11 @@
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="52"/>
-      <c r="B14" s="49"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="52"/>
       <c r="C14" s="16"/>
       <c r="D14" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E14" s="17">
         <v>2</v>
@@ -1725,11 +1725,11 @@
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="52"/>
-      <c r="B15" s="49"/>
+      <c r="A15" s="50"/>
+      <c r="B15" s="52"/>
       <c r="C15" s="16"/>
       <c r="D15" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E15" s="17">
         <v>1</v>
@@ -1741,11 +1741,11 @@
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="52"/>
-      <c r="B16" s="49"/>
+      <c r="A16" s="50"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="16"/>
       <c r="D16" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E16" s="17">
         <v>1</v>
@@ -1757,8 +1757,8 @@
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="52"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="50"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="16"/>
       <c r="D17" s="17" t="s">
         <v>41</v>

</xml_diff>